<commit_message>
Debug and CP problems
</commit_message>
<xml_diff>
--- a/SDE Sheets/DSA-280.xlsx
+++ b/SDE Sheets/DSA-280.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DSA\SDE Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2980E1C-2CCB-4AFC-ACEA-F71528CCBBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5B95DF-170D-4109-B496-1911EBE7C60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="328">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1027,7 +1027,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1153,6 +1153,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1177,10 +1184,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1218,8 +1226,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1438,8 +1448,8 @@
   </sheetPr>
   <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2021,8 +2031,11 @@
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="23" t="s">
         <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.2">
@@ -2291,6 +2304,9 @@
       <c r="B78" s="10" t="s">
         <v>82</v>
       </c>
+      <c r="C78" t="s">
+        <v>327</v>
+      </c>
       <c r="F78" s="3" t="s">
         <v>10</v>
       </c>
@@ -2302,6 +2318,9 @@
       <c r="B79" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="C79" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="80" spans="1:8" ht="15">
       <c r="A80" s="4" t="s">
@@ -2310,6 +2329,9 @@
       <c r="B80" s="10" t="s">
         <v>84</v>
       </c>
+      <c r="C80" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="81" spans="1:7" ht="13.2">
       <c r="A81" s="4" t="s">
@@ -2318,6 +2340,9 @@
       <c r="B81" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="C81" t="s">
+        <v>327</v>
+      </c>
       <c r="F81" s="4" t="s">
         <v>10</v>
       </c>
@@ -2351,6 +2376,9 @@
       <c r="B84" s="6" t="s">
         <v>87</v>
       </c>
+      <c r="C84" t="s">
+        <v>327</v>
+      </c>
       <c r="D84" s="4" t="s">
         <v>10</v>
       </c>
@@ -2379,6 +2407,9 @@
       <c r="B86" s="11" t="s">
         <v>89</v>
       </c>
+      <c r="C86" t="s">
+        <v>327</v>
+      </c>
       <c r="F86" s="4" t="s">
         <v>10</v>
       </c>
@@ -2419,6 +2450,9 @@
       </c>
       <c r="B90" s="11" t="s">
         <v>93</v>
+      </c>
+      <c r="C90" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15">
@@ -2505,6 +2539,9 @@
       <c r="B100" s="15" t="s">
         <v>101</v>
       </c>
+      <c r="C100" t="s">
+        <v>327</v>
+      </c>
       <c r="F100" s="4" t="s">
         <v>10</v>
       </c>
@@ -2637,6 +2674,9 @@
       <c r="B112" s="9" t="s">
         <v>113</v>
       </c>
+      <c r="C112" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="113" spans="1:8" ht="13.2">
       <c r="A113" s="4" t="s">
@@ -2656,6 +2696,9 @@
       <c r="B114" s="9" t="s">
         <v>115</v>
       </c>
+      <c r="C114" t="s">
+        <v>327</v>
+      </c>
       <c r="H114" s="4" t="s">
         <v>10</v>
       </c>
@@ -2677,6 +2720,9 @@
       </c>
       <c r="B116" s="9" t="s">
         <v>117</v>
+      </c>
+      <c r="C116" t="s">
+        <v>327</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>10</v>

</xml_diff>